<commit_message>
Cleared up selectors. Integration testing of individual workflows
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEB914D-CA27-4350-89EB-959FB18E5FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50898FF4-6994-4E07-84CF-1CAE8CE92472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>DispositioningWorkdayQueue</t>
+  </si>
+  <si>
+    <t>WorkdayURL</t>
+  </si>
+  <si>
+    <t>https://impl.workday.com/wday/authgwy/okgov2/login.html</t>
   </si>
 </sst>
 </file>
@@ -257,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -297,7 +303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -403,7 +409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -545,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,7 +562,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -657,7 +663,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
exception handling for individual flows integrated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50898FF4-6994-4E07-84CF-1CAE8CE92472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CA9FB4-9A8F-4CE1-BBAC-1BD1EE566BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>https://impl.workday.com/wday/authgwy/okgov2/login.html</t>
+  </si>
+  <si>
+    <t>ProcessToKill</t>
+  </si>
+  <si>
+    <t>MSEDGE</t>
   </si>
 </sst>
 </file>
@@ -562,7 +568,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -671,7 +677,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Removed warnings in analyze project
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CA9FB4-9A8F-4CE1-BBAC-1BD1EE566BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD89CC3E-FB4C-45C4-A47A-CC3952C8B323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -190,6 +190,18 @@
   </si>
   <si>
     <t>MSEDGE</t>
+  </si>
+  <si>
+    <t>OfferStage</t>
+  </si>
+  <si>
+    <t>HireStage</t>
+  </si>
+  <si>
+    <t>Offer</t>
+  </si>
+  <si>
+    <t>Ready for Hire</t>
   </si>
 </sst>
 </file>
@@ -565,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -685,8 +697,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1672,7 +1698,6 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2847,7 +2872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Development completed for External transfer type
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD89CC3E-FB4C-45C4-A47A-CC3952C8B323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735507CB-A6FF-4B42-9508-DEBB543504F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -159,15 +159,9 @@
     <t>HiringManagerTemplatePath</t>
   </si>
   <si>
-    <t>C:\Users\56382C\Documents\Hiring Manager Template.docx</t>
-  </si>
-  <si>
     <t>WelcomeEmailTemplatePath</t>
   </si>
   <si>
-    <t>C:\Users\56382C\Documents\WelcomeEmailTemplate.docx</t>
-  </si>
-  <si>
     <t>EmailAccount</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer</t>
   </si>
   <si>
-    <t>DispositioningWorkdayQueue</t>
-  </si>
-  <si>
     <t>WorkdayURL</t>
   </si>
   <si>
@@ -202,6 +193,51 @@
   </si>
   <si>
     <t>Ready for Hire</t>
+  </si>
+  <si>
+    <t>O365AppID</t>
+  </si>
+  <si>
+    <t>O365TenantID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationID</t>
+  </si>
+  <si>
+    <t>Shared_O365TenantID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>O365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>C:\Users\56382C\Documents\Hiring Manager Template.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\56382C\Documents\Welcome Email Template.xlsx</t>
+  </si>
+  <si>
+    <t>ExternalTransferCurrency</t>
+  </si>
+  <si>
+    <t>ExternalTransferFrequency</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>CompCodeOverride</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_NHC_WD_Performer_Queue</t>
   </si>
 </sst>
 </file>
@@ -253,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -262,6 +298,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,7 +619,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -630,7 +669,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -640,7 +679,9 @@
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
@@ -651,7 +692,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -662,77 +703,119 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="5">
+        <v>8810</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2873,7 +2956,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Added sharepoint list activities
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A548B120-0BEA-4BC7-9AFE-8606E7079FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B131176-E100-48EE-A96A-86BF53FDDC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -244,13 +244,28 @@
   </si>
   <si>
     <t>P004_SP003_090_NHC_WD_ApprovalStat_Performer_Queue</t>
+  </si>
+  <si>
+    <t>NHC_SharepointURL</t>
+  </si>
+  <si>
+    <t>NHC_SharepointListName</t>
+  </si>
+  <si>
+    <t>DOH_ColumnIndex</t>
+  </si>
+  <si>
+    <t>New Hire Employee Details</t>
+  </si>
+  <si>
+    <t>https://officemgmtentserv.sharepoint.com/sites/NewHireCommunication</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -274,6 +289,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -292,10 +313,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,8 +330,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -625,7 +649,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -816,9 +840,30 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="5">
+        <v>8</v>
+      </c>
+    </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1796,8 +1841,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1" xr:uid="{DB4C3F9B-032B-4124-B024-173A7DF7D657}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Code Review Comments added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312B59ED-56C8-4B6E-B85F-3F903D7F8F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB43F5E-88FA-4C65-B1B2-D5899C492680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -326,6 +326,72 @@
   </si>
   <si>
     <t>RetryScopeAttempts</t>
+  </si>
+  <si>
+    <t>ExceptionEmail</t>
+  </si>
+  <si>
+    <t>BusinessExceptionEmail</t>
+  </si>
+  <si>
+    <t>SE_1</t>
+  </si>
+  <si>
+    <t>Unable to login to Workday Application</t>
+  </si>
+  <si>
+    <t>BE_1</t>
+  </si>
+  <si>
+    <t>Unable to find JR in Workday – "&lt;JR Number&gt;"</t>
+  </si>
+  <si>
+    <t>BE_2</t>
+  </si>
+  <si>
+    <t>Invalid Job Transfer Type</t>
+  </si>
+  <si>
+    <t>SE_2</t>
+  </si>
+  <si>
+    <t>Unable to find Hire Task for the employee in inbox</t>
+  </si>
+  <si>
+    <t>SE_3</t>
+  </si>
+  <si>
+    <t>Unable to update employee details in hire task in inbox</t>
+  </si>
+  <si>
+    <t>SE_4</t>
+  </si>
+  <si>
+    <t>Unable to update employee salary details in hire task in inbox</t>
+  </si>
+  <si>
+    <t>SE_5</t>
+  </si>
+  <si>
+    <t>Unable to submit disposition in workday</t>
+  </si>
+  <si>
+    <t>BE_3</t>
+  </si>
+  <si>
+    <t>Unable to find DOH value for the employee in sharepoint list</t>
+  </si>
+  <si>
+    <t>SE_6</t>
+  </si>
+  <si>
+    <t>Unable to find Change Job Task for the employee in inbox</t>
+  </si>
+  <si>
+    <t>RuntimeLocalFolderPath</t>
+  </si>
+  <si>
+    <t>C:\Users\&lt;Username&gt;\Documents\NHC DispositionWorkday</t>
   </si>
 </sst>
 </file>
@@ -393,7 +459,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -407,17 +473,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -738,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -955,59 +1012,143 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A23" s="7" t="s">
+      <c r="A23" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="132" customHeight="1">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A25" s="7" t="s">
+      <c r="A25" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2206,7 +2347,7 @@
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" s="11"/>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Made internal transfer type as BE
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6EAAD4-836F-4AE5-97AF-5A3581FA2434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B97D2E-DDE3-41EB-9CCC-7D92D3868815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="140">
   <si>
     <t>Name</t>
   </si>
@@ -225,18 +225,12 @@
     <t>SystemException_EmailSubject</t>
   </si>
   <si>
-    <t>The Automation &lt;ProcessName&gt; encountered a system exception.</t>
-  </si>
-  <si>
     <t>SystemException_EmailBody</t>
   </si>
   <si>
     <t>BusinessException_EmailSubject</t>
   </si>
   <si>
-    <t>The Automation &lt;ProcessName&gt; encountered a business exception.</t>
-  </si>
-  <si>
     <t>BusinessException_EmailBody</t>
   </si>
   <si>
@@ -267,21 +261,12 @@
     <t>SE_2</t>
   </si>
   <si>
-    <t>Unable to find Hire Task for the employee in inbox</t>
-  </si>
-  <si>
     <t>SE_3</t>
   </si>
   <si>
-    <t>Unable to update employee details in hire task in inbox</t>
-  </si>
-  <si>
     <t>SE_4</t>
   </si>
   <si>
-    <t>Unable to update employee salary details in hire task in inbox</t>
-  </si>
-  <si>
     <t>SE_5</t>
   </si>
   <si>
@@ -291,15 +276,9 @@
     <t>BE_3</t>
   </si>
   <si>
-    <t>Unable to find DOH value for the employee in sharepoint list</t>
-  </si>
-  <si>
     <t>SE_6</t>
   </si>
   <si>
-    <t>Unable to find Change Job Task for the employee in inbox</t>
-  </si>
-  <si>
     <t>RuntimeLocalFolderPath</t>
   </si>
   <si>
@@ -400,6 +379,24 @@
   </si>
   <si>
     <t>Unable to find Home image in the workday</t>
+  </si>
+  <si>
+    <t>SE_EmailCC</t>
+  </si>
+  <si>
+    <t>BE_EmailCC</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_SE_EmailCC</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_BE_EmailCC</t>
+  </si>
+  <si>
+    <t>SystemExceptionEmail</t>
+  </si>
+  <si>
+    <t>System Exception - HR New Hire Communication Automation - &lt;ExceptionDetail&gt;</t>
   </si>
   <si>
     <t>Hi Team,&lt;BR&gt;
@@ -408,29 +405,17 @@
 &lt;BR&gt;
 &lt;B&gt;Process Name:&lt;/B&gt; &lt;ProcessName&gt;&lt;BR&gt; 
 &lt;B&gt;Process Execution End Time:&lt;/B&gt; &lt;MM/DD/YYYY HH:MM AM/PM&gt;&lt;BR&gt; 
-&lt;B&gt;Process Status:&lt;/B&gt; &lt;SystemException&gt;&lt;BR&gt;
+&lt;B&gt;Exception Detail:&lt;/B&gt; &lt;SystemException&gt;&lt;BR&gt;
 &lt;BR&gt;
 &lt;B&gt;Execution Details:&lt;/B&gt; &lt;ProcessName&gt; has encountered a system exception due to &lt;SystemException&gt;. Please see the attached screenshot of the application issue the automation ran into. Please process manually or restart the process once the issue has been resolved.
 &lt;BR&gt;&lt;BR&gt;
-This is a system generated email, please do not reply back to this email.
-&lt;BR&gt;
+Note: This is a system generated email, please do not reply back to this email. If you have any questions, please reach out to your HR contact or to &lt;HR Email&gt;
+&lt;BR&gt;&lt;BR&gt;
 Regards,&lt;BR&gt; 
 New Hire Communication Automation</t>
   </si>
   <si>
-    <t>SE_EmailCC</t>
-  </si>
-  <si>
-    <t>BE_EmailCC</t>
-  </si>
-  <si>
-    <t>P004_SP003_090_SE_EmailCC</t>
-  </si>
-  <si>
-    <t>P004_SP003_090_BE_EmailCC</t>
-  </si>
-  <si>
-    <t>SystemExceptionEmail</t>
+    <t>Business Exception - HR New Hire Communication Automation - &lt;ExceptionDetail&gt;</t>
   </si>
   <si>
     <t>Hi Team,&lt;BR&gt;
@@ -439,14 +424,53 @@
 &lt;BR&gt;
 &lt;B&gt;Process Name:&lt;/B&gt; &lt;ProcessName&gt;&lt;BR&gt; 
 &lt;B&gt;Process Execution End Time:&lt;/B&gt; &lt;MM/DD/YYYY HH:MM AM/PM&gt;&lt;BR&gt; 
-&lt;B&gt;Process Status:&lt;/B&gt; &lt;BusinessException&gt;&lt;BR&gt;
+&lt;B&gt;Exception Detail:&lt;/B&gt; &lt;BusinessException&gt;&lt;BR&gt;
 &lt;BR&gt;
 Please investigate this matter and process this transaction manually.&lt;BR&gt;
 &lt;BR&gt;
-This is a system generated email, please do not reply back to this email.
-&lt;BR&gt;
+Note: This is a system generated email, please do not reply back to this email. If you have any questions, please reach out to your HR contact or to &lt;HR Email&gt;
+&lt;BR&gt;&lt;BR&gt;
 Regards,&lt;BR&gt; 
 New Hire Communication Automation</t>
+  </si>
+  <si>
+    <t>HR_Email</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_HREmail</t>
+  </si>
+  <si>
+    <t>StaffingAction</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_StaffingAction</t>
+  </si>
+  <si>
+    <t>ChangeReason</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_ChangeReason</t>
+  </si>
+  <si>
+    <t>BE_4</t>
+  </si>
+  <si>
+    <t>Candidate is of internal transfer type</t>
+  </si>
+  <si>
+    <t>Date of Hire value for the candidate is empty for more than 3 days in sharepoint list</t>
+  </si>
+  <si>
+    <t>Unable to find Change Job Task for the candidate in inbox</t>
+  </si>
+  <si>
+    <t>Unable to find Hire Task for the candidate in inbox</t>
+  </si>
+  <si>
+    <t>Unable to update candidate details in hire task in inbox</t>
+  </si>
+  <si>
+    <t>Unable to update candidate salary details in hire task in inbox</t>
   </si>
 </sst>
 </file>
@@ -543,9 +567,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -583,7 +607,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -689,7 +713,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -831,7 +855,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -842,7 +866,7 @@
   <dimension ref="A1:Z978"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -926,116 +950,116 @@
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="132" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
         <v>54</v>
@@ -1043,29 +1067,36 @@
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2256,7 +2287,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -3241,7 +3272,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3293,10 +3324,10 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3304,10 +3335,10 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3315,10 +3346,10 @@
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3326,10 +3357,10 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3337,10 +3368,10 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3348,10 +3379,10 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
@@ -3359,10 +3390,10 @@
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -3370,10 +3401,10 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -3381,10 +3412,10 @@
         <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -3392,10 +3423,10 @@
         <v>53</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -3403,10 +3434,10 @@
         <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -3414,10 +3445,10 @@
         <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -3425,10 +3456,10 @@
         <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -3436,103 +3467,133 @@
         <v>59</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
         <v>127</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
         <v>129</v>
       </c>
-      <c r="C23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="B25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
CR to add building details in  queue
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5843B168-BBD6-4410-95B6-FE7FFAF3B5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10BF849-AF07-4208-BA19-44BECF45D828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,27 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Assets!$A$1:$D$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Assets!$A$1:$D$27</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -186,15 +199,9 @@
     <t>ExternalTransferCurrency</t>
   </si>
   <si>
-    <t>ExternalTransferFrequency</t>
-  </si>
-  <si>
     <t>CompCodeOverride</t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>P004_SP003_090_NHC_WD_Performer_Queue</t>
   </si>
   <si>
@@ -294,16 +301,10 @@
     <t>OrchestratorFolder</t>
   </si>
   <si>
-    <t>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</t>
-  </si>
-  <si>
     <t>P004_SP003_090_OfferStageListValue</t>
   </si>
   <si>
     <t>P004_SP003_090_HireStageListValue</t>
-  </si>
-  <si>
-    <t>P004_SP003_090_FrequencyExternalTransfer</t>
   </si>
   <si>
     <t>P004_SP003_090_CurrencyExternalTransfer</t>
@@ -464,49 +465,61 @@
     <t>P004_Shared_090_WorkdayURL</t>
   </si>
   <si>
+    <t>P004_Shared_090_SharepointURL</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_EmailAccount</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SharepointListName</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SE_Email</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_BE_Email</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_LocalRootFolder</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SE_EmailCC</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_BE_EmailCC</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_HREmail</t>
+  </si>
+  <si>
+    <t>Status_ColumnDisplayName</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_Status_ColumnDisplayName</t>
+  </si>
+  <si>
+    <t>ExternalTransferFrequencyRegular</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_FrequencyExternalTransfer_Regular</t>
+  </si>
+  <si>
+    <t>ExternalTransferFrequencyTemp</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_FrequencyExternalTransfer_Temporary</t>
+  </si>
+  <si>
+    <t>Shared_O365TenantID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationSecret</t>
+  </si>
+  <si>
     <t>DEV/P004_NewHireCommunication</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_SharepointURL</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_EmailAccount</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_O365AppID</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_O365TenantID</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_O365ApplicationSecret</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_SharepointListName</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_SE_Email</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_BE_Email</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_LocalRootFolder</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_SE_EmailCC</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_BE_EmailCC</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_HREmail</t>
-  </si>
-  <si>
-    <t>Status_ColumnDisplayName</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_Status_ColumnDisplayName</t>
   </si>
 </sst>
 </file>
@@ -908,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -959,7 +972,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -970,7 +983,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -990,175 +1003,197 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="132" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1">
       <c r="A20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
+        <v>85</v>
+      </c>
+      <c r="B20" t="str">
+        <f>B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>149</v>
+      </c>
+    </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2303,7 +2338,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2312,7 +2347,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -2320,7 +2355,7 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -2328,7 +2363,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -2336,7 +2371,7 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22">
         <v>0.1</v>
@@ -2344,7 +2379,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -3326,10 +3361,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3381,10 +3416,11 @@
         <v>43</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+      <c r="C2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3392,10 +3428,11 @@
         <v>45</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" t="s">
-        <v>136</v>
+        <v>131</v>
+      </c>
+      <c r="C3" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3403,10 +3440,11 @@
         <v>46</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="C4" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3414,76 +3452,83 @@
         <v>47</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" t="s">
-        <v>136</v>
+        <v>88</v>
+      </c>
+      <c r="C6" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>145</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1">
+        <v>146</v>
+      </c>
+      <c r="C7" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" t="s">
-        <v>136</v>
+        <v>144</v>
+      </c>
+      <c r="C8" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" t="s">
-        <v>88</v>
+        <v>52</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="C10" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" t="s">
-        <v>88</v>
+        <v>55</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -3491,199 +3536,195 @@
         <v>56</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" t="s">
-        <v>88</v>
+        <v>134</v>
+      </c>
+      <c r="C12" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" t="s">
-        <v>136</v>
+      <c r="B13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C14" t="s">
-        <v>136</v>
+      <c r="C14" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" t="s">
-        <v>88</v>
+        <v>105</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>136</v>
+      </c>
+      <c r="C16" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="C17" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C18" t="s">
-        <v>136</v>
+        <v>92</v>
+      </c>
+      <c r="C18" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C19" t="s">
-        <v>136</v>
+        <v>94</v>
+      </c>
+      <c r="C19" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C20" t="s">
-        <v>88</v>
+      <c r="C20" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" t="s">
-        <v>88</v>
+        <v>138</v>
+      </c>
+      <c r="C21" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" t="s">
-        <v>88</v>
+        <v>139</v>
+      </c>
+      <c r="C22" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C23" t="s">
-        <v>136</v>
+        <v>140</v>
+      </c>
+      <c r="C23" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" t="s">
-        <v>136</v>
+        <v>110</v>
+      </c>
+      <c r="C24" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C25" t="s">
-        <v>136</v>
+      <c r="C25" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" t="s">
-        <v>88</v>
+        <v>126</v>
+      </c>
+      <c r="C26" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>129</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" t="s">
-        <v>88</v>
-      </c>
-    </row>
+        <v>128</v>
+      </c>
+      <c r="C27" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4653,8 +4694,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Involved to select BOT account in case SSO fails
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000AE148-2B3C-49E6-8795-8FA1178A687C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4B0B43-66D1-4F4C-8BCB-F2A5F617D73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="154">
   <si>
     <t>Name</t>
   </si>
@@ -517,6 +517,15 @@
   </si>
   <si>
     <t>Shared_O365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>BOTCredentialAssetName</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_BOT_Credentials</t>
+  </si>
+  <si>
+    <t>ProcessAssetFolderPath</t>
   </si>
   <si>
     <t>PROD/P004_NewHireCommunication</t>
@@ -921,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -983,7 +992,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -1194,8 +1203,23 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>152</v>
+      </c>
+      <c r="B31" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+      </c>
+    </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
@@ -3364,7 +3388,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Log In screen change
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDisposition_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4B0B43-66D1-4F4C-8BCB-F2A5F617D73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9604EB95-422D-4AAB-9286-1622488BD246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,7 +528,7 @@
     <t>ProcessAssetFolderPath</t>
   </si>
   <si>
-    <t>PROD/P004_NewHireCommunication</t>
+    <t>DEV/P004_NewHireCommunication</t>
   </si>
 </sst>
 </file>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="B20" t="str">
         <f>B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="B31" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3444,7 +3444,7 @@
       </c>
       <c r="C2" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="C3" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3468,7 +3468,7 @@
       </c>
       <c r="C4" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3480,7 +3480,7 @@
       </c>
       <c r="C5" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3492,7 +3492,7 @@
       </c>
       <c r="C6" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="C7" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3516,7 +3516,7 @@
       </c>
       <c r="C8" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -3528,7 +3528,7 @@
       </c>
       <c r="C9" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="C10" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="C11" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -3564,7 +3564,7 @@
       </c>
       <c r="C12" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -3576,7 +3576,7 @@
       </c>
       <c r="C13" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -3588,7 +3588,7 @@
       </c>
       <c r="C14" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -3600,7 +3600,7 @@
       </c>
       <c r="C15" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -3612,7 +3612,7 @@
       </c>
       <c r="C16" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
@@ -3624,7 +3624,7 @@
       </c>
       <c r="C17" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="C18" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="C19" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -3660,7 +3660,7 @@
       </c>
       <c r="C20" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -3672,7 +3672,7 @@
       </c>
       <c r="C21" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -3684,7 +3684,7 @@
       </c>
       <c r="C22" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -3696,7 +3696,7 @@
       </c>
       <c r="C23" t="str">
         <f>Settings!B3</f>
-        <v>PROD/P004_NewHireCommunication</v>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="C24" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -3720,7 +3720,7 @@
       </c>
       <c r="C25" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
@@ -3732,7 +3732,7 @@
       </c>
       <c r="C26" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -3744,7 +3744,7 @@
       </c>
       <c r="C27" t="str">
         <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
-        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>